<commit_message>
Change of ovality scaling
</commit_message>
<xml_diff>
--- a/data/process_format/Process_PLA.xlsx
+++ b/data/process_format/Process_PLA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/process_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDE80E0-7F38-3B41-BAE3-5AB45DFD579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE91FC9-3220-634E-80AE-D62F8FD94F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="21260" windowHeight="17400" activeTab="1" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
+    <workbookView xWindow="12100" yWindow="540" windowWidth="21260" windowHeight="17400" activeTab="1" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
   </bookViews>
   <sheets>
     <sheet name="process_params" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -125,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -142,7 +153,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +560,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,8 +621,8 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="8">
-        <v>1E-3</v>
+      <c r="F3" s="7">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -632,7 +642,7 @@
         <f>process_params!B4</f>
         <v>29.693999999999999</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ovality threshold scaling
</commit_message>
<xml_diff>
--- a/data/process_format/Process_PLA.xlsx
+++ b/data/process_format/Process_PLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/process_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE91FC9-3220-634E-80AE-D62F8FD94F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D02562-E3EB-4449-931E-720E8C04797B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12100" yWindow="540" windowWidth="21260" windowHeight="17400" activeTab="1" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
   </bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>